<commit_message>
Game Testing on 14th Feb
</commit_message>
<xml_diff>
--- a/quest.xlsx
+++ b/quest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,96 @@
   </si>
   <si>
     <t>louvre</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Question Title</t>
+  </si>
+  <si>
+    <t>Decrypt the Anagram</t>
+  </si>
+  <si>
+    <t>themonalisa</t>
+  </si>
+  <si>
+    <t>An anagram is a type of word play, the result of rearranging the letters of a word or phrase to produce a new word or phrase, using all the original letters exactly once; for example orchestra can be rearranged into carthorse. "Oh, Lame Saint!"</t>
+  </si>
+  <si>
+    <t>Question Description</t>
+  </si>
+  <si>
+    <t>leonardodavinci</t>
+  </si>
+  <si>
+    <t>An anagram is a type of word play, the result of rearranging the letters of a word or phrase to produce a new word or phrase, using all the original letters exactly once; for example orchestra can be rearranged into carthorse. "O, Draconian Devil"</t>
+  </si>
+  <si>
+    <t>An anagram is a type of word play, the result of rearranging the letters of a word or phrase to produce a new word or phrase, using all the original letters exactly once; for example orchestra can be rearranged into carthorse. "So dark the con of man"</t>
+  </si>
+  <si>
+    <t>madonnaoftherocks</t>
+  </si>
+  <si>
+    <t>An anagram is a type of word play, the result of rearranging the letters of a word or phrase to produce a new word or phrase, using all the original letters exactly once; for example orchestra can be rearranged into carthorse. "I am a weakish speller"</t>
+  </si>
+  <si>
+    <t>williamshakespeare</t>
+  </si>
+  <si>
+    <t>An anagram is a type of word play, the result of rearranging the letters of a word or phrase to produce a new word or phrase, using all the original letters exactly once; for example orchestra can be rearranged into carthorse. "Tom Marvolo Riddle"</t>
+  </si>
+  <si>
+    <t>iamlordvoldemort</t>
+  </si>
+  <si>
+    <r>
+      <t>The invention of the printing press by a German goldsmith (1398–1468) is widely regarded as the single most important event of the second millennium, and is one of the defining moments of the Renaissance. The </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Printing Revolution</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> which it sparked throughout Europe, worked as a modern "agent of change" in the transformation of medieval society. Who is the German Goldsmith?</t>
+    </r>
+  </si>
+  <si>
+    <t>printingpress.png</t>
+  </si>
+  <si>
+    <t>johannesgutenberg</t>
+  </si>
+  <si>
+    <t>This Empire had been one of the first Middle Eastern states (that extended into Europe, making them the first European state as well) to effectively use gunpowder weapons and used them to great effect conquering much of the Middle East, North Africa, and the Balkans. In the 17th century, the state began to stagnate as more modern technologies and strategies were not adopted. Which Empire are we talking about? (Hint : 'Only the name of empire'</t>
+  </si>
+  <si>
+    <t>ottoman</t>
+  </si>
+  <si>
+    <t>gunpowder.png</t>
+  </si>
+  <si>
+    <t>florenze.jpg</t>
+  </si>
+  <si>
+    <t>city.jpg</t>
+  </si>
+  <si>
+    <t>florence</t>
+  </si>
+  <si>
+    <t>david</t>
   </si>
   <si>
     <r>
@@ -55,113 +145,15 @@
         <color rgb="FF444444"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>, probably the world’s most famous painting. It was painted sometime between 1503 and 1506, when da Vinci was living in Florence, and it now hangs in</t>
+      <t>, probably the world’s most famous painting. It was painted sometime between 1503 and 1506, when da Vinci was living in Florence, and it now hangs in Paris, where it remains an object of pilgrimage in the 21st century. The poplar panel shows evidence of warping and was stabilized in 1951 with the addition of an oak frame and in 1970 with four vertical braces. Dovetails also were added, to prevent the widening of a small crack visible near the centre of the upper edge of the painting. &lt;span class="clue&gt;"In which Museum does Mona Lisa Hang?&lt;/span&gt;</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF444444"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Paris, where it remains an object of pilgrimage in the 21st century. The poplar panel shows evidence of warping and was stabilized in 1951 with the addition of an oak frame and in 1970 with four vertical braces. Dovetails also were added, to prevent the widening of a small crack visible near the centre of the upper edge of the painting.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Question Title</t>
-  </si>
-  <si>
-    <t>Decrypt the Anagram</t>
-  </si>
-  <si>
-    <t>themonalisa</t>
-  </si>
-  <si>
-    <t>An anagram is a type of word play, the result of rearranging the letters of a word or phrase to produce a new word or phrase, using all the original letters exactly once; for example orchestra can be rearranged into carthorse. "Oh, Lame Saint!"</t>
-  </si>
-  <si>
-    <t>Question Description</t>
-  </si>
-  <si>
-    <t>leonardodavinci</t>
-  </si>
-  <si>
-    <t>An anagram is a type of word play, the result of rearranging the letters of a word or phrase to produce a new word or phrase, using all the original letters exactly once; for example orchestra can be rearranged into carthorse. "O, Draconian Devil"</t>
-  </si>
-  <si>
-    <t>An anagram is a type of word play, the result of rearranging the letters of a word or phrase to produce a new word or phrase, using all the original letters exactly once; for example orchestra can be rearranged into carthorse. "So dark the con of man"</t>
-  </si>
-  <si>
-    <t>madonnaoftherocks</t>
-  </si>
-  <si>
-    <t>An anagram is a type of word play, the result of rearranging the letters of a word or phrase to produce a new word or phrase, using all the original letters exactly once; for example orchestra can be rearranged into carthorse. "I am a weakish speller"</t>
-  </si>
-  <si>
-    <t>williamshakespeare</t>
-  </si>
-  <si>
-    <t>An anagram is a type of word play, the result of rearranging the letters of a word or phrase to produce a new word or phrase, using all the original letters exactly once; for example orchestra can be rearranged into carthorse. "Tom Marvolo Riddle"</t>
-  </si>
-  <si>
-    <t>iamlordvoldemort</t>
-  </si>
-  <si>
-    <r>
-      <t>The invention of the printing press by a German goldsmith (1398–1468) is widely regarded as the single most important event of the second millennium, and is one of the defining moments of the Renaissance. The </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF0B0080"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Printing Revolution</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t> which it sparked throughout Europe, worked as a modern "agent of change" in the transformation of medieval society. Who is the German Goldsmith?</t>
-    </r>
-  </si>
-  <si>
-    <t>printingpress.png</t>
-  </si>
-  <si>
-    <t>johannesgutenberg</t>
-  </si>
-  <si>
-    <t>This Empire had been one of the first Middle Eastern states (that extended into Europe, making them the first European state as well) to effectively use gunpowder weapons and used them to great effect conquering much of the Middle East, North Africa, and the Balkans. In the 17th century, the state began to stagnate as more modern technologies and strategies were not adopted. Which Empire are we talking about? (Hint : 'Only the name of empire'</t>
-  </si>
-  <si>
-    <t>ottoman</t>
-  </si>
-  <si>
-    <t>gunpowder.png</t>
-  </si>
-  <si>
-    <t>florenze.jpg</t>
-  </si>
-  <si>
-    <t>city.jpg</t>
-  </si>
-  <si>
-    <t>florence</t>
-  </si>
-  <si>
-    <t>david</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -195,6 +187,22 @@
       <color rgb="FF0B0080"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -213,8 +221,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -237,7 +247,9 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -570,7 +582,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -587,21 +599,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="153">
+    <row r="2" spans="1:4" ht="170">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -609,99 +621,100 @@
     </row>
     <row r="3" spans="1:4" ht="45">
       <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45">
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45">
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45">
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45">
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="80">
       <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="96">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>